<commit_message>
extraction effiency stats corrected
</commit_message>
<xml_diff>
--- a/figures/4_heatmap/data/sputum_extraction_summary.xlsx
+++ b/figures/4_heatmap/data/sputum_extraction_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaneykalinich/Documents/PGCoE/github/pgcoe_pipeline/figures/4_heatmap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43C9A32-A3C9-D046-920F-1F1727E6B36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B92FBC4-E0DF-5F42-A060-C15F85B915DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="394">
   <si>
     <t>Lab details</t>
   </si>
@@ -1316,6 +1316,12 @@
   </si>
   <si>
     <t>group</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -2144,10 +2150,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FCBDCD-8DAE-AB40-A1EF-769E24854A98}">
   <dimension ref="A1:AL61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="L58" sqref="L58"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42:J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2313,7 +2319,7 @@
         <v>383</v>
       </c>
       <c r="J2" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K2" s="60" t="s">
         <v>383</v>
@@ -2429,7 +2435,7 @@
         <v>383</v>
       </c>
       <c r="J3" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K3" s="60" t="s">
         <v>383</v>
@@ -2545,7 +2551,7 @@
         <v>383</v>
       </c>
       <c r="J4" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K4" s="60" t="s">
         <v>383</v>
@@ -2663,7 +2669,7 @@
         <v>383</v>
       </c>
       <c r="J5" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K5" s="60" t="s">
         <v>383</v>
@@ -2781,7 +2787,7 @@
         <v>383</v>
       </c>
       <c r="J6" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K6" s="60" t="s">
         <v>383</v>
@@ -2899,7 +2905,7 @@
         <v>383</v>
       </c>
       <c r="J7" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K7" s="60" t="s">
         <v>383</v>
@@ -3017,7 +3023,7 @@
         <v>383</v>
       </c>
       <c r="J8" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K8" s="60" t="s">
         <v>383</v>
@@ -3135,7 +3141,7 @@
         <v>383</v>
       </c>
       <c r="J9" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K9" s="60" t="s">
         <v>383</v>
@@ -3251,7 +3257,7 @@
         <v>383</v>
       </c>
       <c r="J10" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K10" s="60" t="s">
         <v>383</v>
@@ -3367,7 +3373,7 @@
         <v>383</v>
       </c>
       <c r="J11" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K11" s="60" t="s">
         <v>383</v>
@@ -3485,7 +3491,7 @@
         <v>383</v>
       </c>
       <c r="J12" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K12" s="60" t="s">
         <v>384</v>
@@ -3601,7 +3607,7 @@
         <v>383</v>
       </c>
       <c r="J13" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K13" s="60" t="s">
         <v>384</v>
@@ -3720,7 +3726,7 @@
         <v>383</v>
       </c>
       <c r="J14" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K14" s="60" t="s">
         <v>384</v>
@@ -3838,7 +3844,7 @@
         <v>383</v>
       </c>
       <c r="J15" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K15" s="60" t="s">
         <v>384</v>
@@ -3954,7 +3960,7 @@
         <v>383</v>
       </c>
       <c r="J16" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K16" s="60" t="s">
         <v>384</v>
@@ -4072,7 +4078,7 @@
         <v>383</v>
       </c>
       <c r="J17" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K17" s="60" t="s">
         <v>384</v>
@@ -4190,7 +4196,7 @@
         <v>383</v>
       </c>
       <c r="J18" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K18" s="60" t="s">
         <v>384</v>
@@ -4308,7 +4314,7 @@
         <v>383</v>
       </c>
       <c r="J19" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K19" s="60" t="s">
         <v>384</v>
@@ -4427,7 +4433,7 @@
         <v>383</v>
       </c>
       <c r="J20" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K20" s="60" t="s">
         <v>384</v>
@@ -4543,7 +4549,7 @@
         <v>383</v>
       </c>
       <c r="J21" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K21" s="60" t="s">
         <v>384</v>
@@ -4658,10 +4664,10 @@
         <v>380</v>
       </c>
       <c r="I22" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J22" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K22" s="60" t="s">
         <v>385</v>
@@ -4777,10 +4783,10 @@
         <v>380</v>
       </c>
       <c r="I23" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J23" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K23" s="60" t="s">
         <v>385</v>
@@ -4895,10 +4901,10 @@
         <v>380</v>
       </c>
       <c r="I24" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J24" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K24" s="60" t="s">
         <v>385</v>
@@ -5013,10 +5019,10 @@
         <v>380</v>
       </c>
       <c r="I25" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J25" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K25" s="60" t="s">
         <v>385</v>
@@ -5134,10 +5140,10 @@
         <v>380</v>
       </c>
       <c r="I26" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J26" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K26" s="60" t="s">
         <v>385</v>
@@ -5252,10 +5258,10 @@
         <v>380</v>
       </c>
       <c r="I27" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J27" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K27" s="60" t="s">
         <v>385</v>
@@ -5370,10 +5376,10 @@
         <v>380</v>
       </c>
       <c r="I28" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J28" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K28" s="60" t="s">
         <v>385</v>
@@ -5489,10 +5495,10 @@
         <v>380</v>
       </c>
       <c r="I29" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J29" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K29" s="60" t="s">
         <v>385</v>
@@ -5607,10 +5613,10 @@
         <v>380</v>
       </c>
       <c r="I30" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J30" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K30" s="60" t="s">
         <v>385</v>
@@ -5725,10 +5731,10 @@
         <v>380</v>
       </c>
       <c r="I31" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J31" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K31" s="60" t="s">
         <v>385</v>
@@ -5846,10 +5852,10 @@
         <v>380</v>
       </c>
       <c r="I32" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J32" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K32" s="60" t="s">
         <v>386</v>
@@ -5967,10 +5973,10 @@
         <v>380</v>
       </c>
       <c r="I33" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J33" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K33" s="60" t="s">
         <v>386</v>
@@ -6085,10 +6091,10 @@
         <v>380</v>
       </c>
       <c r="I34" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J34" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K34" s="60" t="s">
         <v>386</v>
@@ -6201,10 +6207,10 @@
         <v>380</v>
       </c>
       <c r="I35" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J35" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K35" s="60" t="s">
         <v>386</v>
@@ -6320,10 +6326,10 @@
         <v>380</v>
       </c>
       <c r="I36" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J36" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K36" s="60" t="s">
         <v>386</v>
@@ -6438,10 +6444,10 @@
         <v>380</v>
       </c>
       <c r="I37" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J37" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K37" s="60" t="s">
         <v>386</v>
@@ -6556,10 +6562,10 @@
         <v>380</v>
       </c>
       <c r="I38" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J38" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K38" s="60" t="s">
         <v>386</v>
@@ -6677,10 +6683,10 @@
         <v>380</v>
       </c>
       <c r="I39" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J39" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K39" s="60" t="s">
         <v>386</v>
@@ -6795,10 +6801,10 @@
         <v>380</v>
       </c>
       <c r="I40" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J40" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K40" s="60" t="s">
         <v>386</v>
@@ -6913,10 +6919,10 @@
         <v>380</v>
       </c>
       <c r="I41" s="60" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J41" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K41" s="60" t="s">
         <v>386</v>
@@ -7031,10 +7037,10 @@
         <v>380</v>
       </c>
       <c r="I42" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J42" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K42" s="60" t="s">
         <v>387</v>
@@ -7086,6 +7092,9 @@
       </c>
       <c r="AC42">
         <v>19.34</v>
+      </c>
+      <c r="AD42">
+        <v>154839.73300000001</v>
       </c>
       <c r="AE42">
         <v>17706088</v>
@@ -7135,10 +7144,10 @@
         <v>380</v>
       </c>
       <c r="I43" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J43" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K43" s="60" t="s">
         <v>387</v>
@@ -7190,6 +7199,9 @@
       </c>
       <c r="AC43">
         <v>18.600000000000001</v>
+      </c>
+      <c r="AD43">
+        <v>256626.25</v>
       </c>
       <c r="AE43">
         <v>23307331</v>
@@ -7239,10 +7251,10 @@
         <v>380</v>
       </c>
       <c r="I44" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J44" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K44" s="60" t="s">
         <v>387</v>
@@ -7294,6 +7306,9 @@
       </c>
       <c r="AC44">
         <v>20.49</v>
+      </c>
+      <c r="AD44">
+        <v>70311.608999999997</v>
       </c>
       <c r="AE44">
         <v>12931029</v>
@@ -7343,10 +7358,10 @@
         <v>380</v>
       </c>
       <c r="I45" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J45" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K45" s="60" t="s">
         <v>387</v>
@@ -7398,6 +7413,9 @@
       </c>
       <c r="AC45">
         <v>20.47</v>
+      </c>
+      <c r="AD45">
+        <v>71332.655100000004</v>
       </c>
       <c r="AE45">
         <v>24006624</v>
@@ -7450,10 +7468,10 @@
         <v>380</v>
       </c>
       <c r="I46" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J46" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K46" s="60" t="s">
         <v>387</v>
@@ -7505,6 +7523,9 @@
       </c>
       <c r="AC46">
         <v>21.68</v>
+      </c>
+      <c r="AD46">
+        <v>31163.203000000001</v>
       </c>
       <c r="AE46">
         <v>12477026</v>
@@ -7554,10 +7575,10 @@
         <v>380</v>
       </c>
       <c r="I47" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J47" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K47" s="60" t="s">
         <v>387</v>
@@ -7609,6 +7630,9 @@
       </c>
       <c r="AC47">
         <v>19.13</v>
+      </c>
+      <c r="AD47">
+        <v>178117.826</v>
       </c>
       <c r="AE47">
         <v>5687659</v>
@@ -7658,10 +7682,10 @@
         <v>380</v>
       </c>
       <c r="I48" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J48" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K48" s="60" t="s">
         <v>387</v>
@@ -7713,6 +7737,9 @@
       </c>
       <c r="AC48">
         <v>26.96</v>
+      </c>
+      <c r="AD48">
+        <v>842.41276200000004</v>
       </c>
       <c r="AE48">
         <v>564341</v>
@@ -7762,10 +7789,10 @@
         <v>380</v>
       </c>
       <c r="I49" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J49" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K49" s="60" t="s">
         <v>387</v>
@@ -7817,6 +7844,9 @@
       </c>
       <c r="AC49">
         <v>20.94</v>
+      </c>
+      <c r="AD49">
+        <v>51807.204700000002</v>
       </c>
       <c r="AE49">
         <v>22396761</v>
@@ -7869,10 +7899,10 @@
         <v>380</v>
       </c>
       <c r="I50" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J50" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K50" s="60" t="s">
         <v>387</v>
@@ -7924,6 +7954,9 @@
       </c>
       <c r="AC50">
         <v>19.43</v>
+      </c>
+      <c r="AD50">
+        <v>145411.677</v>
       </c>
       <c r="AE50">
         <v>17533361</v>
@@ -7973,10 +8006,10 @@
         <v>380</v>
       </c>
       <c r="I51" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J51" s="60" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="K51" s="60" t="s">
         <v>387</v>
@@ -8028,6 +8061,9 @@
       </c>
       <c r="AC51">
         <v>20.83</v>
+      </c>
+      <c r="AD51">
+        <v>55663.396099999998</v>
       </c>
       <c r="AE51">
         <v>9460128</v>
@@ -8077,10 +8113,10 @@
         <v>381</v>
       </c>
       <c r="I52" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J52" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K52" s="60" t="s">
         <v>388</v>
@@ -8132,6 +8168,9 @@
       </c>
       <c r="AC52">
         <v>18.66</v>
+      </c>
+      <c r="AD52">
+        <v>245859.18799999999</v>
       </c>
       <c r="AE52">
         <v>21871679</v>
@@ -8181,10 +8220,10 @@
         <v>381</v>
       </c>
       <c r="I53" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J53" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K53" s="60" t="s">
         <v>388</v>
@@ -8236,6 +8275,9 @@
       </c>
       <c r="AC53">
         <v>18.32</v>
+      </c>
+      <c r="AD53">
+        <v>310986.31400000001</v>
       </c>
       <c r="AE53">
         <v>35475733</v>
@@ -8285,10 +8327,10 @@
         <v>381</v>
       </c>
       <c r="I54" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J54" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K54" s="60" t="s">
         <v>388</v>
@@ -8340,6 +8382,9 @@
       </c>
       <c r="AC54">
         <v>20.77</v>
+      </c>
+      <c r="AD54">
+        <v>58066.633900000001</v>
       </c>
       <c r="AE54">
         <v>8582413</v>
@@ -8389,10 +8434,10 @@
         <v>381</v>
       </c>
       <c r="I55" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J55" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K55" s="60" t="s">
         <v>388</v>
@@ -8444,6 +8489,9 @@
       </c>
       <c r="AC55">
         <v>20.420000000000002</v>
+      </c>
+      <c r="AD55">
+        <v>73951.044599999994</v>
       </c>
       <c r="AE55">
         <v>7179363</v>
@@ -8493,10 +8541,10 @@
         <v>381</v>
       </c>
       <c r="I56" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J56" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K56" s="60" t="s">
         <v>388</v>
@@ -8548,6 +8596,9 @@
       </c>
       <c r="AC56">
         <v>22.06</v>
+      </c>
+      <c r="AD56">
+        <v>24021.507399999999</v>
       </c>
       <c r="AE56">
         <v>7746608</v>
@@ -8597,10 +8648,10 @@
         <v>381</v>
       </c>
       <c r="I57" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J57" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K57" s="60" t="s">
         <v>388</v>
@@ -8652,6 +8703,9 @@
       </c>
       <c r="AC57">
         <v>18.59</v>
+      </c>
+      <c r="AD57">
+        <v>257744.58499999999</v>
       </c>
       <c r="AE57">
         <v>7083106</v>
@@ -8701,10 +8755,10 @@
         <v>381</v>
       </c>
       <c r="I58" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J58" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K58" s="60" t="s">
         <v>388</v>
@@ -8756,6 +8810,9 @@
       </c>
       <c r="AC58">
         <v>26.98</v>
+      </c>
+      <c r="AD58">
+        <v>828.87104899999997</v>
       </c>
       <c r="AE58">
         <v>515535</v>
@@ -8805,10 +8862,10 @@
         <v>381</v>
       </c>
       <c r="I59" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J59" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K59" s="60" t="s">
         <v>388</v>
@@ -8860,6 +8917,9 @@
       </c>
       <c r="AC59">
         <v>21.59</v>
+      </c>
+      <c r="AD59">
+        <v>33249.812100000003</v>
       </c>
       <c r="AE59">
         <v>867329</v>
@@ -8912,10 +8972,10 @@
         <v>381</v>
       </c>
       <c r="I60" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J60" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K60" s="60" t="s">
         <v>388</v>
@@ -8967,6 +9027,9 @@
       </c>
       <c r="AC60">
         <v>18.27</v>
+      </c>
+      <c r="AD60">
+        <v>321880.962</v>
       </c>
       <c r="AE60">
         <v>27341768</v>
@@ -9016,10 +9079,10 @@
         <v>381</v>
       </c>
       <c r="I61" s="60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J61" s="60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="K61" s="60" t="s">
         <v>388</v>
@@ -9071,6 +9134,9 @@
       </c>
       <c r="AC61">
         <v>20.59</v>
+      </c>
+      <c r="AD61">
+        <v>65844.383600000001</v>
       </c>
       <c r="AE61">
         <v>12772952</v>

</xml_diff>